<commit_message>
new file mobile checklist
</commit_message>
<xml_diff>
--- a/Form_testing_(Checklist).xlsx
+++ b/Form_testing_(Checklist).xlsx
@@ -1626,6 +1626,15 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1634,15 +1643,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3660,7 +3660,10 @@
   <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4521,7 +4524,10 @@
   <dimension ref="A1:Z38"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5370,7 +5376,10 @@
   <dimension ref="A1:Z71"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G22" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6901,7 +6910,10 @@
   <dimension ref="A1:Z59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8022,7 +8034,10 @@
   <dimension ref="A1:Z59"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8928,7 +8943,7 @@
   </sheetPr>
   <dimension ref="A2:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21:K21"/>
     </sheetView>
   </sheetViews>
@@ -8984,251 +8999,257 @@
       <c r="B7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="49" t="s">
+      <c r="C7" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
     </row>
     <row r="8" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7">
         <v>1</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="45" t="s">
         <v>388</v>
       </c>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
     </row>
     <row r="9" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7">
         <v>2</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="45" t="s">
         <v>389</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
     </row>
     <row r="10" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>3</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="45" t="s">
         <v>390</v>
       </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
     </row>
     <row r="11" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="50" t="s">
+      <c r="C11" s="46" t="s">
         <v>391</v>
       </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
     </row>
     <row r="12" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>5</v>
       </c>
-      <c r="C12" s="48" t="s">
+      <c r="C12" s="45" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="48"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
     </row>
     <row r="13" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="7">
         <v>6</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="45" t="s">
         <v>392</v>
       </c>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="48"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
     </row>
     <row r="14" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="7">
         <v>7</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="45" t="s">
         <v>393</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="48"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
     </row>
     <row r="15" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7">
         <v>8</v>
       </c>
-      <c r="C15" s="50" t="s">
+      <c r="C15" s="46" t="s">
         <v>394</v>
       </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="46"/>
     </row>
     <row r="16" spans="2:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="7">
         <v>9</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="45" t="s">
         <v>395</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>10</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="45" t="s">
         <v>396</v>
       </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="48"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
       <c r="B18" s="29">
         <v>11</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="48" t="s">
         <v>406</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="46"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
-      <c r="K18" s="47"/>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="49"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="50"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="29">
         <v>12</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="48" t="s">
         <v>407</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="47"/>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
+      <c r="F19" s="49"/>
+      <c r="G19" s="49"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="50"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="29">
         <v>13</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="48" t="s">
         <v>408</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="47"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="50"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="29">
         <v>14</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="48" t="s">
         <v>409</v>
       </c>
-      <c r="D21" s="46"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="47"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="50"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C18:K18"/>
+    <mergeCell ref="C19:K19"/>
+    <mergeCell ref="C20:K20"/>
+    <mergeCell ref="C21:K21"/>
+    <mergeCell ref="C16:K16"/>
+    <mergeCell ref="C17:K17"/>
     <mergeCell ref="C14:K14"/>
     <mergeCell ref="C15:K15"/>
     <mergeCell ref="C12:K12"/>
@@ -9241,12 +9262,6 @@
     <mergeCell ref="C9:K9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="C11:K11"/>
-    <mergeCell ref="C18:K18"/>
-    <mergeCell ref="C19:K19"/>
-    <mergeCell ref="C20:K20"/>
-    <mergeCell ref="C21:K21"/>
-    <mergeCell ref="C16:K16"/>
-    <mergeCell ref="C17:K17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1" display="http://itcareer.pythonanywhere.com/"/>

</xml_diff>